<commit_message>
Cleared existing results, added repast results
(To spreadsheet)
</commit_message>
<xml_diff>
--- a/single machine/Results.xlsx
+++ b/single machine/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" tabRatio="594" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" tabRatio="594"/>
   </bookViews>
   <sheets>
     <sheet name="Problem Scale" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
   <si>
     <t>Width</t>
   </si>
@@ -67,13 +67,7 @@
     <t>~Neighbourhood Size</t>
   </si>
   <si>
-    <t>int divison -_-</t>
-  </si>
-  <si>
-    <t>not clean of background processes during execution</t>
-  </si>
-  <si>
-    <t>Total Runtime (ms)</t>
+    <t>Total Runtime (s)</t>
   </si>
 </sst>
 </file>
@@ -168,6 +162,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -323,82 +318,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1.3296687009999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3293426509999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4113469240000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.890015381</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5227583010000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2815832519999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4750925289999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.868917969</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7971728520000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9806035160000004</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.1846215820000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.8701787109999994</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.461048827999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.402624023</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.600598633000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.81025</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22.069751953000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26.338525391000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31.749654296999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>39.234289062999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>50.756660156000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>63.797164062999997</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>81.460984374999995</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>103.31897656300001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>126.844820313</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>153.56476562500001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -438,82 +433,197 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>3.12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.6470000000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6280000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.571999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.265999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.722999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.662999999999997</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39.515000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>73.647999999999996</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72.509</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>94.644999999999996</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>147.935</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>127.40600000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>169.40100000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>210.35</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>263.85899999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>391.904</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>329.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>428.892</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>477.01799999999997</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>739.25400000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>776.42899999999997</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>714.52800000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>868.25099999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1007.169</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1170.1420000000001</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Problem Scale'!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>REPAST</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Problem Scale'!$K$4:$K$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3040000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5180000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.545000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.108999000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47.221001000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62.945999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.262000999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>122.225998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>161.865005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>212.658997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260.58300800000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>324.55801400000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>400.71798699999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>479.17001299999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>597.85497999999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>710.92498799999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>815.86602800000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>936.43902600000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1077.26001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1259.2810059999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1431.520996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1611.5920410000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1833.7060550000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2046.395996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -529,11 +639,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="216672008"/>
-        <c:axId val="216672392"/>
+        <c:axId val="31547184"/>
+        <c:axId val="215703072"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="216672008"/>
+        <c:axId val="31547184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,6 +705,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -661,7 +772,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216672392"/>
+        <c:crossAx val="215703072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -670,7 +781,7 @@
         <c:majorTimeUnit val="years"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="216672392"/>
+        <c:axId val="215703072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,6 +828,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -777,7 +889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216672008"/>
+        <c:crossAx val="31547184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -801,6 +913,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1758,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,10 +1953,13 @@
         <v>1250</v>
       </c>
       <c r="I4">
-        <v>1.3296687009999999</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>3.12</v>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>2.98</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1873,10 +1989,13 @@
         <v>2160</v>
       </c>
       <c r="I5">
-        <v>1.3293426509999999</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>5.6470000000000002</v>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>5.3040000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1906,10 +2025,13 @@
         <v>3430</v>
       </c>
       <c r="I6">
-        <v>1.4113469240000001</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>7.6280000000000001</v>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>8.5180000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1939,10 +2061,13 @@
         <v>5120</v>
       </c>
       <c r="I7">
-        <v>1.890015381</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>13.571999999999999</v>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>13.666</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1972,10 +2097,13 @@
         <v>7290</v>
       </c>
       <c r="I8">
-        <v>2.5227583010000001</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>19.265999999999998</v>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>20.545000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2005,10 +2133,13 @@
         <v>10000</v>
       </c>
       <c r="I9">
-        <v>3.2815832519999999</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>26.722999999999999</v>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>29.108999000000001</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2038,10 +2169,13 @@
         <v>13310</v>
       </c>
       <c r="I10">
-        <v>3.4750925289999999</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>34.662999999999997</v>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>47.221001000000001</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2071,10 +2205,13 @@
         <v>17280</v>
       </c>
       <c r="I11">
-        <v>4.868917969</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>39.515000000000001</v>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>62.945999</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2104,10 +2241,13 @@
         <v>21970</v>
       </c>
       <c r="I12">
-        <v>5.7971728520000001</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>73.647999999999996</v>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>90.262000999999998</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2137,10 +2277,13 @@
         <v>27440</v>
       </c>
       <c r="I13">
-        <v>6.9806035160000004</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>72.509</v>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>122.225998</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2170,10 +2313,13 @@
         <v>33750</v>
       </c>
       <c r="I14">
-        <v>8.1846215820000001</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>94.644999999999996</v>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>161.865005</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2203,10 +2349,13 @@
         <v>40960</v>
       </c>
       <c r="I15">
-        <v>9.8701787109999994</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>147.935</v>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>212.658997</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2236,13 +2385,16 @@
         <v>49130</v>
       </c>
       <c r="I16">
-        <v>11.461048827999999</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>127.40600000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>260.58300800000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>180</v>
       </c>
@@ -2269,13 +2421,16 @@
         <v>58320</v>
       </c>
       <c r="I17">
-        <v>13.402624023</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>169.40100000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>324.55801400000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>190</v>
       </c>
@@ -2302,13 +2457,16 @@
         <v>68590</v>
       </c>
       <c r="I18">
-        <v>15.600598633000001</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>210.35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>400.71798699999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>200</v>
       </c>
@@ -2335,13 +2493,16 @@
         <v>80000</v>
       </c>
       <c r="I19">
-        <v>17.81025</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>263.85899999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>479.17001299999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>210</v>
       </c>
@@ -2368,13 +2529,16 @@
         <v>92610</v>
       </c>
       <c r="I20">
-        <v>22.069751953000001</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>391.904</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>597.85497999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>220</v>
       </c>
@@ -2401,13 +2565,16 @@
         <v>106480</v>
       </c>
       <c r="I21">
-        <v>26.338525391000001</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>329.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>710.92498799999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>230</v>
       </c>
@@ -2434,13 +2601,16 @@
         <v>121670</v>
       </c>
       <c r="I22">
-        <v>31.749654296999999</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>428.892</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>815.86602800000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>240</v>
       </c>
@@ -2467,13 +2637,16 @@
         <v>138240</v>
       </c>
       <c r="I23">
-        <v>39.234289062999999</v>
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>477.01799999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>936.43902600000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>250</v>
       </c>
@@ -2500,13 +2673,16 @@
         <v>156250</v>
       </c>
       <c r="I24">
-        <v>50.756660156000002</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>739.25400000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>1077.26001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>260</v>
       </c>
@@ -2533,13 +2709,16 @@
         <v>175760</v>
       </c>
       <c r="I25">
-        <v>63.797164062999997</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>776.42899999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>1259.2810059999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>270</v>
       </c>
@@ -2566,13 +2745,16 @@
         <v>196830</v>
       </c>
       <c r="I26">
-        <v>81.460984374999995</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>714.52800000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>1431.520996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>280</v>
       </c>
@@ -2599,13 +2781,16 @@
         <v>219520</v>
       </c>
       <c r="I27">
-        <v>103.31897656300001</v>
+        <v>0</v>
       </c>
       <c r="J27">
-        <v>868.25099999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1611.5920410000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>290</v>
       </c>
@@ -2632,13 +2817,16 @@
         <v>243890</v>
       </c>
       <c r="I28">
-        <v>126.844820313</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>1007.169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1833.7060550000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>300</v>
       </c>
@@ -2665,10 +2853,13 @@
         <v>270000</v>
       </c>
       <c r="I29">
-        <v>153.56476562500001</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>1170.1420000000001</v>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>2046.395996</v>
       </c>
     </row>
   </sheetData>
@@ -2679,10 +2870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L19"/>
+  <dimension ref="A2:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L18"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2749,7 +2940,7 @@
         <v>0.01</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1.0000000000000001E-5</v>
@@ -2769,13 +2960,10 @@
       </c>
       <c r="I4">
         <f>B4*PI()*POWER(2*C4,G4)</f>
-        <v>848.23001646924422</v>
-      </c>
-      <c r="J4">
-        <v>31.110082031000001</v>
-      </c>
-      <c r="K4">
-        <v>1279</v>
+        <v>0.25132741228718347</v>
+      </c>
+      <c r="L4">
+        <v>23.976998999999999</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2786,7 +2974,7 @@
         <v>0.01</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>1.0000000000000001E-5</v>
@@ -2806,13 +2994,10 @@
       </c>
       <c r="I5">
         <f t="shared" ref="I5:I18" si="1">B5*PI()*POWER(2*C5,G5)</f>
-        <v>689.64241931603146</v>
-      </c>
-      <c r="J5">
-        <v>30.829562500000002</v>
-      </c>
-      <c r="K5">
-        <v>1221</v>
+        <v>2.0106192982974678</v>
+      </c>
+      <c r="L5">
+        <v>25.709</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2823,7 +3008,7 @@
         <v>0.01</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>1.0000000000000001E-5</v>
@@ -2843,13 +3028,10 @@
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>552.16632479494206</v>
-      </c>
-      <c r="J6">
-        <v>30.516906250000002</v>
-      </c>
-      <c r="K6">
-        <v>1165</v>
+        <v>6.7858401317539538</v>
+      </c>
+      <c r="L6">
+        <v>27.111999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2860,7 +3042,7 @@
         <v>0.01</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>1.0000000000000001E-5</v>
@@ -2880,13 +3062,10 @@
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>434.29376843225305</v>
-      </c>
-      <c r="J7">
-        <v>17.638400391000001</v>
-      </c>
-      <c r="K7">
-        <v>832</v>
+        <v>16.084954386379742</v>
+      </c>
+      <c r="L7">
+        <v>28.657</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2897,7 +3076,7 @@
         <v>0.01</v>
       </c>
       <c r="C8">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>1.0000000000000001E-5</v>
@@ -2917,13 +3096,10 @@
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>334.5167857542412</v>
-      </c>
-      <c r="J8">
-        <v>17.40084375</v>
-      </c>
-      <c r="K8">
-        <v>801</v>
+        <v>31.415926535897935</v>
+      </c>
+      <c r="L8">
+        <v>30.372999</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2934,7 +3110,7 @@
         <v>0.01</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>1.0000000000000001E-5</v>
@@ -2954,13 +3130,10 @@
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>251.32741228718348</v>
-      </c>
-      <c r="J9">
-        <v>17.293359375000001</v>
-      </c>
-      <c r="K9">
-        <v>611</v>
+        <v>54.286721054031631</v>
+      </c>
+      <c r="L9">
+        <v>40.341999000000001</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2971,7 +3144,7 @@
         <v>0.01</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>1.0000000000000001E-5</v>
@@ -2991,13 +3164,10 @@
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>183.21768355735676</v>
-      </c>
-      <c r="J10">
-        <v>10.647922852000001</v>
-      </c>
-      <c r="K10">
-        <v>470</v>
+        <v>86.205302414503933</v>
+      </c>
+      <c r="L10">
+        <v>35.536999000000002</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3030,11 +3200,8 @@
         <f t="shared" si="1"/>
         <v>128.67963509103794</v>
       </c>
-      <c r="J11">
-        <v>7.1979970700000004</v>
-      </c>
-      <c r="K11">
-        <v>323</v>
+      <c r="L11">
+        <v>43.945</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3045,7 +3212,7 @@
         <v>0.01</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>1.0000000000000001E-5</v>
@@ -3065,13 +3232,10 @@
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>86.205302414503933</v>
-      </c>
-      <c r="J12">
-        <v>4.8720610349999998</v>
-      </c>
-      <c r="K12">
-        <v>216</v>
+        <v>183.21768355735676</v>
+      </c>
+      <c r="L12">
+        <v>45.256000999999998</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3082,7 +3246,7 @@
         <v>0.01</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <v>1.0000000000000001E-5</v>
@@ -3102,13 +3266,10 @@
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>54.286721054031631</v>
-      </c>
-      <c r="J13">
-        <v>3.6434091799999999</v>
-      </c>
-      <c r="K13">
-        <v>126</v>
+        <v>251.32741228718348</v>
+      </c>
+      <c r="L13">
+        <v>53.710999000000001</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3119,7 +3280,7 @@
         <v>0.01</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D14">
         <v>1.0000000000000001E-5</v>
@@ -3139,13 +3300,10 @@
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
-        <v>31.415926535897935</v>
-      </c>
-      <c r="J14">
-        <v>3.209141357</v>
-      </c>
-      <c r="K14">
-        <v>78</v>
+        <v>334.5167857542412</v>
+      </c>
+      <c r="L14">
+        <v>52.525002000000001</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3156,7 +3314,7 @@
         <v>0.01</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D15">
         <v>1.0000000000000001E-5</v>
@@ -3176,13 +3334,10 @@
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
-        <v>16.084954386379742</v>
-      </c>
-      <c r="J15">
-        <v>1.909305298</v>
-      </c>
-      <c r="K15">
-        <v>61</v>
+        <v>434.29376843225305</v>
+      </c>
+      <c r="L15">
+        <v>63.992001000000002</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3193,7 +3348,7 @@
         <v>0.01</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D16">
         <v>1.0000000000000001E-5</v>
@@ -3213,16 +3368,13 @@
       </c>
       <c r="I16">
         <f t="shared" si="1"/>
-        <v>6.7858401317539538</v>
-      </c>
-      <c r="J16">
-        <v>1.4079912109999999</v>
-      </c>
-      <c r="K16">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>552.16632479494206</v>
+      </c>
+      <c r="L16">
+        <v>80.417998999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>100</v>
       </c>
@@ -3230,7 +3382,7 @@
         <v>0.01</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>1.0000000000000001E-5</v>
@@ -3250,16 +3402,13 @@
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
-        <v>2.0106192982974678</v>
-      </c>
-      <c r="J17">
-        <v>1.1389998779999999</v>
-      </c>
-      <c r="K17">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>689.64241931603146</v>
+      </c>
+      <c r="L17">
+        <v>80.948997000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>100</v>
       </c>
@@ -3267,7 +3416,7 @@
         <v>0.01</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D18">
         <v>1.0000000000000001E-5</v>
@@ -3287,21 +3436,10 @@
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
-        <v>0.25132741228718347</v>
-      </c>
-      <c r="J18">
-        <v>1.497269897</v>
-      </c>
-      <c r="K18">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J19" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" t="s">
-        <v>13</v>
+        <v>848.23001646924422</v>
+      </c>
+      <c r="L18">
+        <v>109.18499799999999</v>
       </c>
     </row>
   </sheetData>
@@ -3313,8 +3451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3324,7 +3462,7 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3395,8 +3533,8 @@
         <f>B4*PI()*POWER(2*C4,G4)</f>
         <v>31.415926535897935</v>
       </c>
-      <c r="J4">
-        <v>360.53537</v>
+      <c r="L4">
+        <v>3.5259999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3429,8 +3567,8 @@
         <f t="shared" ref="I5:I11" si="1">B5*PI()*POWER(2*C5,G5)</f>
         <v>31.415926535897935</v>
       </c>
-      <c r="J5">
-        <v>336.588165</v>
+      <c r="L5">
+        <v>3.323</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3463,8 +3601,8 @@
         <f t="shared" si="1"/>
         <v>31.415926535897935</v>
       </c>
-      <c r="J6">
-        <v>322.64254799999998</v>
+      <c r="L6">
+        <v>3.4009999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3497,8 +3635,8 @@
         <f t="shared" si="1"/>
         <v>31.415926535897935</v>
       </c>
-      <c r="J7">
-        <v>320.503784</v>
+      <c r="L7">
+        <v>3.5419999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3531,8 +3669,8 @@
         <f t="shared" si="1"/>
         <v>31.415926535897935</v>
       </c>
-      <c r="J8">
-        <v>320.39111300000002</v>
+      <c r="L8">
+        <v>3.2610000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3565,8 +3703,8 @@
         <f t="shared" si="1"/>
         <v>31.415926535897935</v>
       </c>
-      <c r="J9">
-        <v>323.15640300000001</v>
+      <c r="L9">
+        <v>3.2450000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3599,8 +3737,8 @@
         <f t="shared" si="1"/>
         <v>31.415926535897935</v>
       </c>
-      <c r="J10">
-        <v>324.22195399999998</v>
+      <c r="L10">
+        <v>3.4009999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3633,8 +3771,8 @@
         <f t="shared" si="1"/>
         <v>31.415926535897935</v>
       </c>
-      <c r="J11">
-        <v>319.39193699999998</v>
+      <c r="L11">
+        <v>3.4169999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3667,8 +3805,8 @@
         <f t="shared" ref="I12" si="3">B12*PI()*POWER(2*C12,G12)</f>
         <v>31.415926535897935</v>
       </c>
-      <c r="J12">
-        <v>319.77529900000002</v>
+      <c r="L12">
+        <v>3.4169999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added most MASON results to spreadsheet.
</commit_message>
<xml_diff>
--- a/single machine/Results.xlsx
+++ b/single machine/Results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\Desktop\circles\single machine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robadob\circles\single machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" tabRatio="594"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" tabRatio="594" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Problem Scale" sheetId="1" r:id="rId1"/>
@@ -199,8 +199,192 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Problem Scale'!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MASON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Problem Scale'!$H$4:$H$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2160</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3430</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7290</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13310</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21970</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27440</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40960</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>58320</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>68590</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>92610</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>106480</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121670</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>138240</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>156250</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>175760</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>196830</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>219520</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>243890</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>270000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Problem Scale'!$J$4:$J$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>7.8159999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.368</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.728000999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.814999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56.097999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75.567001000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>102.05500000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>136.875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180.10200499999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>238.86799600000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>302.32900999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>462.307007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>556.78100600000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>796.50598100000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>931.85199</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1231.154053</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1631.3570560000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1888.1960449999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2313.4370119999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2481.7150879999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'Problem Scale'!$I$3</c:f>
@@ -401,121 +585,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Problem Scale'!$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MASON</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Problem Scale'!$J$4:$J$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
@@ -541,6 +610,93 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Problem Scale'!$H$4:$H$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2160</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3430</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7290</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13310</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21970</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27440</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40960</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>58320</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>68590</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>92610</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>106480</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121670</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>138240</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>156250</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>175760</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>196830</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>219520</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>243890</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>270000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Problem Scale'!$K$4:$K$29</c:f>
@@ -639,11 +795,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="229999520"/>
-        <c:axId val="230023056"/>
+        <c:axId val="205126752"/>
+        <c:axId val="205125968"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="229999520"/>
+        <c:axId val="205126752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,7 +928,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230023056"/>
+        <c:crossAx val="205125968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -781,7 +937,7 @@
         <c:majorTimeUnit val="years"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="230023056"/>
+        <c:axId val="205125968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,7 +1045,1459 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229999520"/>
+        <c:crossAx val="205126752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Circles Benchmark vs Neighbourhood Size</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'~Neighbourhood Scale'!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MASON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'~Neighbourhood Scale'!$I$4:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.25132741228718347</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0106192982974678</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7858401317539538</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.084954386379742</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.415926535897935</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.286721054031631</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>86.205302414503933</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.67963509103794</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>183.21768355735676</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>251.32741228718348</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>334.5167857542412</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>434.29376843225305</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>552.16632479494206</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>689.64241931603146</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>848.23001646924422</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'~Neighbourhood Scale'!$K$4:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>26.863001000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.509998000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.652000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62.915000999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78.155997999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.142998000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119.05999799999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>144.533997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>190.46099899999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>217.94799800000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>256.71499599999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>277.18099999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>398.20700099999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>432.61999500000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>430.31201199999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'~Neighbourhood Scale'!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FLAMEGPU Partitioning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'~Neighbourhood Scale'!$I$4:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.25132741228718347</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0106192982974678</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7858401317539538</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.084954386379742</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.415926535897935</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.286721054031631</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>86.205302414503933</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.67963509103794</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>183.21768355735676</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>251.32741228718348</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>334.5167857542412</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>434.29376843225305</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>552.16632479494206</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>689.64241931603146</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>848.23001646924422</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'~Neighbourhood Scale'!$J$4:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.7817329099999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.078756592</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3511909179999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3128330080000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7136484379999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0065546879999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.513123047000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.476560547</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.660400391</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.406080077999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.544294921999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.357056641</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23.299552733999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23.428734375000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.322919922000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'~Neighbourhood Scale'!$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>REPAST</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'~Neighbourhood Scale'!$I$4:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.25132741228718347</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0106192982974678</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7858401317539538</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.084954386379742</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.415926535897935</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.286721054031631</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>86.205302414503933</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.67963509103794</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>183.21768355735676</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>251.32741228718348</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>334.5167857542412</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>434.29376843225305</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>552.16632479494206</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>689.64241931603146</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>848.23001646924422</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'~Neighbourhood Scale'!$L$4:$L$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>23.976998999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.709</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.111999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.657</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.372999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.341999000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.536999000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.945</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.256000999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>53.710999000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.525002000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63.992001000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>80.417998999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80.948997000000006</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>109.18499799999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="447623376"/>
+        <c:axId val="447621416"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="447623376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Agents</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="447621416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="years"/>
+        <c:majorUnit val="18"/>
+        <c:majorTimeUnit val="years"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="447621416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Iteration Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="447623376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Circles Benchmark vs Entropy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Entropy!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MASON</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Entropy!$K$4:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8.4860000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2059999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.7050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2520000000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5960000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.3149999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.2210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.2370000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Entropy!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FLAMEGPU Partitioning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Entropy!$J$4:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.78130944800000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76337078899999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77297155799999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75933013900000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.76136505099999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77788977100000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.77518804900000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75468469199999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.74390893599999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Entropy!$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>REPAST</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Entropy!$L$4:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.5259999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.323</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4009999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5419999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2610000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4009999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4169999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4169999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="509280408"/>
+        <c:axId val="509283152"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="509280408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Agents</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509283152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="years"/>
+        <c:majorUnit val="18"/>
+        <c:majorTimeUnit val="years"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="509283152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Iteration Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509280408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1020,7 +2628,1189 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1575,21 +4365,95 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1869,10 +4733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K29"/>
+  <dimension ref="A2:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1956,7 +4820,7 @@
         <v>1.5141464840000001</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>7.8159999999999998</v>
       </c>
       <c r="K4">
         <v>2.98</v>
@@ -1985,14 +4849,14 @@
         <v>3</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H29" si="0">_xlfn.FLOOR.MATH(POWER(A5,G5)*B5)</f>
+        <f t="shared" ref="H5:J29" si="0">_xlfn.FLOOR.MATH(POWER(A5,G5)*B5)</f>
         <v>2160</v>
       </c>
       <c r="I5">
         <v>1.6465123290000001</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>14.368</v>
       </c>
       <c r="K5">
         <v>5.3040000000000003</v>
@@ -2028,7 +4892,7 @@
         <v>1.8888035889999999</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>23.728000999999999</v>
       </c>
       <c r="K6">
         <v>8.5180000000000007</v>
@@ -2064,7 +4928,7 @@
         <v>3.1863854979999999</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>37.814999</v>
       </c>
       <c r="K7">
         <v>13.666</v>
@@ -2100,7 +4964,7 @@
         <v>5.1155761719999999</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>56.097999999999999</v>
       </c>
       <c r="K8">
         <v>20.545000000000002</v>
@@ -2136,7 +5000,7 @@
         <v>7.6742490229999998</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>75.567001000000005</v>
       </c>
       <c r="K9">
         <v>29.108999000000001</v>
@@ -2172,7 +5036,7 @@
         <v>8.9056552730000007</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>102.05500000000001</v>
       </c>
       <c r="K10">
         <v>47.221001000000001</v>
@@ -2208,7 +5072,7 @@
         <v>13.941623047</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>136.875</v>
       </c>
       <c r="K11">
         <v>62.945999</v>
@@ -2244,7 +5108,7 @@
         <v>18.335865234</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>180.10200499999999</v>
       </c>
       <c r="K12">
         <v>90.262000999999998</v>
@@ -2280,7 +5144,7 @@
         <v>24.529195312999999</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>238.86799600000001</v>
       </c>
       <c r="K13">
         <v>122.225998</v>
@@ -2316,7 +5180,7 @@
         <v>31.386851563</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>302.32900999999998</v>
       </c>
       <c r="K14">
         <v>161.865005</v>
@@ -2352,7 +5216,7 @@
         <v>41.593425781000001</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>462.307007</v>
       </c>
       <c r="K15">
         <v>212.658997</v>
@@ -2388,7 +5252,7 @@
         <v>51.811347656000002</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>556.78100600000005</v>
       </c>
       <c r="K16">
         <v>260.58300800000001</v>
@@ -2424,7 +5288,7 @@
         <v>65.555007813000003</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>796.50598100000002</v>
       </c>
       <c r="K17">
         <v>324.55801400000001</v>
@@ -2460,7 +5324,7 @@
         <v>81.061992188000005</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>931.85199</v>
       </c>
       <c r="K18">
         <v>400.71798699999999</v>
@@ -2496,7 +5360,7 @@
         <v>98.289351562999997</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>1231.154053</v>
       </c>
       <c r="K19">
         <v>479.17001299999998</v>
@@ -2532,7 +5396,7 @@
         <v>120.353351563</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1631.3570560000001</v>
       </c>
       <c r="K20">
         <v>597.85497999999995</v>
@@ -2568,7 +5432,7 @@
         <v>144.46899999999999</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>1888.1960449999999</v>
       </c>
       <c r="K21">
         <v>710.92498799999998</v>
@@ -2604,7 +5468,7 @@
         <v>174.66145312500001</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>2313.4370119999999</v>
       </c>
       <c r="K22">
         <v>815.86602800000003</v>
@@ -2640,7 +5504,7 @@
         <v>215.19103125000001</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>2481.7150879999999</v>
       </c>
       <c r="K23">
         <v>936.43902600000001</v>
@@ -2675,9 +5539,6 @@
       <c r="I24">
         <v>273.65828125000002</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
       <c r="K24">
         <v>1077.26001</v>
       </c>
@@ -2711,9 +5572,6 @@
       <c r="I25">
         <v>346.10393749999997</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
       <c r="K25">
         <v>1259.2810059999999</v>
       </c>
@@ -2747,9 +5605,6 @@
       <c r="I26">
         <v>435.43337500000001</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
       <c r="K26">
         <v>1431.520996</v>
       </c>
@@ -2783,9 +5638,6 @@
       <c r="I27">
         <v>553.20487500000002</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
       <c r="K27">
         <v>1611.5920410000001</v>
       </c>
@@ -2819,9 +5671,6 @@
       <c r="I28">
         <v>708.90762500000005</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
       <c r="K28">
         <v>1833.7060550000001</v>
       </c>
@@ -2855,11 +5704,198 @@
       <c r="I29">
         <v>916.73137499999996</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
       <c r="K29">
         <v>2046.395996</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>1250</v>
+      </c>
+      <c r="I34">
+        <v>7.8159999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>2160</v>
+      </c>
+      <c r="I35">
+        <v>14.368</v>
+      </c>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>3430</v>
+      </c>
+      <c r="I36">
+        <v>23.728000999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>5120</v>
+      </c>
+      <c r="I37">
+        <v>37.814999</v>
+      </c>
+    </row>
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>7290</v>
+      </c>
+      <c r="I38">
+        <v>56.097999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>10000</v>
+      </c>
+      <c r="I39">
+        <v>75.567001000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>13310</v>
+      </c>
+      <c r="I40">
+        <v>102.05500000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>17280</v>
+      </c>
+      <c r="I41">
+        <v>136.875</v>
+      </c>
+    </row>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>21970</v>
+      </c>
+      <c r="I42">
+        <v>180.10200499999999</v>
+      </c>
+    </row>
+    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>27440</v>
+      </c>
+      <c r="I43">
+        <v>238.86799600000001</v>
+      </c>
+    </row>
+    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>33750</v>
+      </c>
+      <c r="I44">
+        <v>302.32900999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>40960</v>
+      </c>
+      <c r="I45">
+        <v>462.307007</v>
+      </c>
+    </row>
+    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>49130</v>
+      </c>
+      <c r="I46">
+        <v>556.78100600000005</v>
+      </c>
+    </row>
+    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>58320</v>
+      </c>
+      <c r="I47">
+        <v>796.50598100000002</v>
+      </c>
+    </row>
+    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>68590</v>
+      </c>
+      <c r="I48">
+        <v>931.85199</v>
+      </c>
+    </row>
+    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>80000</v>
+      </c>
+      <c r="I49">
+        <v>1231.154053</v>
+      </c>
+    </row>
+    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>92610</v>
+      </c>
+      <c r="I50">
+        <v>1631.3570560000001</v>
+      </c>
+    </row>
+    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>106480</v>
+      </c>
+      <c r="I51">
+        <v>1888.1960449999999</v>
+      </c>
+    </row>
+    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>121670</v>
+      </c>
+      <c r="I52">
+        <v>2313.4370119999999</v>
+      </c>
+    </row>
+    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>138240</v>
+      </c>
+      <c r="I53">
+        <v>2481.7150879999999</v>
+      </c>
+    </row>
+    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>156250</v>
+      </c>
+    </row>
+    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H55">
+        <v>175760</v>
+      </c>
+    </row>
+    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <v>196830</v>
+      </c>
+    </row>
+    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H57">
+        <v>219520</v>
+      </c>
+    </row>
+    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>243890</v>
+      </c>
+    </row>
+    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>270000</v>
       </c>
     </row>
   </sheetData>
@@ -2870,10 +5906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L18"/>
+  <dimension ref="A2:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23:K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2965,6 +6001,9 @@
       <c r="J4">
         <v>1.7817329099999999</v>
       </c>
+      <c r="K4">
+        <v>26.863001000000001</v>
+      </c>
       <c r="L4">
         <v>23.976998999999999</v>
       </c>
@@ -3002,6 +6041,9 @@
       <c r="J5">
         <v>2.078756592</v>
       </c>
+      <c r="K5">
+        <v>42.509998000000003</v>
+      </c>
       <c r="L5">
         <v>25.709</v>
       </c>
@@ -3039,6 +6081,9 @@
       <c r="J6">
         <v>3.3511909179999999</v>
       </c>
+      <c r="K6">
+        <v>51.652000000000001</v>
+      </c>
       <c r="L6">
         <v>27.111999999999998</v>
       </c>
@@ -3076,6 +6121,9 @@
       <c r="J7">
         <v>5.3128330080000001</v>
       </c>
+      <c r="K7">
+        <v>62.915000999999997</v>
+      </c>
       <c r="L7">
         <v>28.657</v>
       </c>
@@ -3113,6 +6161,9 @@
       <c r="J8">
         <v>7.7136484379999999</v>
       </c>
+      <c r="K8">
+        <v>78.155997999999997</v>
+      </c>
       <c r="L8">
         <v>30.372999</v>
       </c>
@@ -3150,6 +6201,9 @@
       <c r="J9">
         <v>9.0065546879999996</v>
       </c>
+      <c r="K9">
+        <v>96.142998000000006</v>
+      </c>
       <c r="L9">
         <v>40.341999000000001</v>
       </c>
@@ -3187,6 +6241,9 @@
       <c r="J10">
         <v>10.513123047000001</v>
       </c>
+      <c r="K10">
+        <v>119.05999799999999</v>
+      </c>
       <c r="L10">
         <v>35.536999000000002</v>
       </c>
@@ -3224,6 +6281,9 @@
       <c r="J11">
         <v>12.476560547</v>
       </c>
+      <c r="K11">
+        <v>144.533997</v>
+      </c>
       <c r="L11">
         <v>43.945</v>
       </c>
@@ -3261,6 +6321,9 @@
       <c r="J12">
         <v>15.660400391</v>
       </c>
+      <c r="K12">
+        <v>190.46099899999999</v>
+      </c>
       <c r="L12">
         <v>45.256000999999998</v>
       </c>
@@ -3298,6 +6361,9 @@
       <c r="J13">
         <v>19.406080077999999</v>
       </c>
+      <c r="K13">
+        <v>217.94799800000001</v>
+      </c>
       <c r="L13">
         <v>53.710999000000001</v>
       </c>
@@ -3335,6 +6401,9 @@
       <c r="J14">
         <v>18.544294921999999</v>
       </c>
+      <c r="K14">
+        <v>256.71499599999999</v>
+      </c>
       <c r="L14">
         <v>52.525002000000001</v>
       </c>
@@ -3372,6 +6441,9 @@
       <c r="J15">
         <v>18.357056641</v>
       </c>
+      <c r="K15">
+        <v>277.18099999999998</v>
+      </c>
       <c r="L15">
         <v>63.992001000000002</v>
       </c>
@@ -3409,6 +6481,9 @@
       <c r="J16">
         <v>23.299552733999999</v>
       </c>
+      <c r="K16">
+        <v>398.20700099999999</v>
+      </c>
       <c r="L16">
         <v>80.417998999999995</v>
       </c>
@@ -3446,6 +6521,9 @@
       <c r="J17">
         <v>23.428734375000001</v>
       </c>
+      <c r="K17">
+        <v>432.61999500000002</v>
+      </c>
       <c r="L17">
         <v>80.948997000000006</v>
       </c>
@@ -3483,12 +6561,136 @@
       <c r="J18">
         <v>24.322919922000001</v>
       </c>
+      <c r="K18">
+        <v>430.31201199999998</v>
+      </c>
       <c r="L18">
         <v>109.18499799999999</v>
       </c>
     </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>0.25132741199999997</v>
+      </c>
+      <c r="K23">
+        <v>23.976998999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>2.0106192979999999</v>
+      </c>
+      <c r="K24">
+        <v>25.709</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>6.7858401319999997</v>
+      </c>
+      <c r="K25">
+        <v>27.111999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>16.08495439</v>
+      </c>
+      <c r="K26">
+        <v>28.657</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>31.415926540000001</v>
+      </c>
+      <c r="K27">
+        <v>30.372999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>54.286721049999997</v>
+      </c>
+      <c r="K28">
+        <v>40.341999000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>86.205302410000002</v>
+      </c>
+      <c r="K29">
+        <v>35.536999000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>128.67963510000001</v>
+      </c>
+      <c r="K30">
+        <v>43.945</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>183.21768359999999</v>
+      </c>
+      <c r="K31">
+        <v>45.256000999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>251.32741229999999</v>
+      </c>
+      <c r="K32">
+        <v>53.710999000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>334.51678579999998</v>
+      </c>
+      <c r="K33">
+        <v>52.525002000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>434.29376839999998</v>
+      </c>
+      <c r="K34">
+        <v>63.992001000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <v>552.16632479999998</v>
+      </c>
+      <c r="K35">
+        <v>80.417998999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <v>689.64241930000003</v>
+      </c>
+      <c r="K36">
+        <v>80.948997000000006</v>
+      </c>
+    </row>
+    <row r="37" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>848.23001650000003</v>
+      </c>
+      <c r="K37">
+        <v>109.18499799999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3496,8 +6698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3581,6 +6783,9 @@
       <c r="J4">
         <v>0.78130944800000002</v>
       </c>
+      <c r="K4">
+        <v>8.4860000000000007</v>
+      </c>
       <c r="L4">
         <v>3.5259999999999998</v>
       </c>
@@ -3618,6 +6823,9 @@
       <c r="J5">
         <v>0.76337078899999999</v>
       </c>
+      <c r="K5">
+        <v>8.2059999999999995</v>
+      </c>
       <c r="L5">
         <v>3.323</v>
       </c>
@@ -3655,6 +6863,9 @@
       <c r="J6">
         <v>0.77297155799999995</v>
       </c>
+      <c r="K6">
+        <v>8.7050000000000001</v>
+      </c>
       <c r="L6">
         <v>3.4009999999999998</v>
       </c>
@@ -3692,6 +6903,9 @@
       <c r="J7">
         <v>0.75933013900000002</v>
       </c>
+      <c r="K7">
+        <v>8.33</v>
+      </c>
       <c r="L7">
         <v>3.5419999999999998</v>
       </c>
@@ -3729,6 +6943,9 @@
       <c r="J8">
         <v>0.76136505099999996</v>
       </c>
+      <c r="K8">
+        <v>8.2520000000000007</v>
+      </c>
       <c r="L8">
         <v>3.2610000000000001</v>
       </c>
@@ -3766,6 +6983,9 @@
       <c r="J9">
         <v>0.77788977100000001</v>
       </c>
+      <c r="K9">
+        <v>8.5960000000000001</v>
+      </c>
       <c r="L9">
         <v>3.2450000000000001</v>
       </c>
@@ -3803,6 +7023,9 @@
       <c r="J10">
         <v>0.77518804900000005</v>
       </c>
+      <c r="K10">
+        <v>8.3149999999999995</v>
+      </c>
       <c r="L10">
         <v>3.4009999999999998</v>
       </c>
@@ -3840,6 +7063,9 @@
       <c r="J11">
         <v>0.75468469199999999</v>
       </c>
+      <c r="K11">
+        <v>8.2210000000000001</v>
+      </c>
       <c r="L11">
         <v>3.4169999999999998</v>
       </c>
@@ -3877,11 +7103,15 @@
       <c r="J12">
         <v>0.74390893599999997</v>
       </c>
+      <c r="K12">
+        <v>8.2370000000000001</v>
+      </c>
       <c r="L12">
         <v>3.4169999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added PCC to results spreadsheet.
</commit_message>
<xml_diff>
--- a/single machine/Results.xlsx
+++ b/single machine/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\Desktop\circles\single machine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robadob\circles\single machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
   <si>
     <t>Width</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Total Runtime (s)</t>
+  </si>
+  <si>
+    <t>Pearson:</t>
+  </si>
+  <si>
+    <t>Pearson 150k+:</t>
   </si>
 </sst>
 </file>
@@ -851,11 +857,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218242488"/>
-        <c:axId val="218242872"/>
+        <c:axId val="350406680"/>
+        <c:axId val="350413736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218242488"/>
+        <c:axId val="350406680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -984,13 +990,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218242872"/>
+        <c:crossAx val="350413736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="18"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218242872"/>
+        <c:axId val="350413736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,7 +1104,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218242488"/>
+        <c:crossAx val="350406680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1571,11 +1577,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218268984"/>
-        <c:axId val="217979224"/>
+        <c:axId val="350405504"/>
+        <c:axId val="350412168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218268984"/>
+        <c:axId val="350405504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1704,13 +1710,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217979224"/>
+        <c:crossAx val="350412168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="18"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="217979224"/>
+        <c:axId val="350412168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1818,7 +1824,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218268984"/>
+        <c:crossAx val="350405504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1949,7 +1955,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2224,11 +2229,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218111520"/>
-        <c:axId val="218111904"/>
+        <c:axId val="350409816"/>
+        <c:axId val="350416872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218111520"/>
+        <c:axId val="350409816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2290,7 +2295,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2357,13 +2361,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218111904"/>
+        <c:crossAx val="350416872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="18"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218111904"/>
+        <c:axId val="350416872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2410,7 +2414,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2471,7 +2474,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218111520"/>
+        <c:crossAx val="350409816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2495,7 +2498,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4709,8 +4711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4720,6 +4722,7 @@
     <col min="4" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
   </cols>
@@ -5698,6 +5701,32 @@
       </c>
       <c r="K29">
         <v>2046.395996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31">
+        <f>PEARSON(H4:H29,I4:I29)</f>
+        <v>0.94983175514954699</v>
+      </c>
+      <c r="J31">
+        <f>PEARSON(H4:H29,J4:J29)</f>
+        <v>0.98906791076451894</v>
+      </c>
+      <c r="K31">
+        <f>PEARSON(H4:H29,K4:K29)</f>
+        <v>0.99795691464180614</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32">
+        <f>PEARSON(H24:H29,I24:I29)</f>
+        <v>0.98995036505789602</v>
       </c>
     </row>
     <row r="34" spans="8:9" x14ac:dyDescent="0.25">
@@ -5900,8 +5929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="H3" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6558,6 +6587,23 @@
       </c>
       <c r="L18">
         <v>109.18499799999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20">
+        <f>PEARSON(I4:I18,J4:J18)</f>
+        <v>0.90496685194058868</v>
+      </c>
+      <c r="K20">
+        <f>PEARSON(I4:I18,K4:K18)</f>
+        <v>0.98551717301605513</v>
+      </c>
+      <c r="L20">
+        <f>PEARSON(I4:I18,L4:L18)</f>
+        <v>0.98457785821354371</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed bug with FLAMEGPU model implementation, reproduced results.
Correct FLAMEGPU model is now ~4-5x faster, will require ammending paper.
</commit_message>
<xml_diff>
--- a/single machine/Results.xlsx
+++ b/single machine/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robadob\circles\single machine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\Desktop\circles\single machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -73,7 +73,7 @@
     <t>Pearson:</t>
   </si>
   <si>
-    <t>Pearson 150k+:</t>
+    <t>Pearson 110k+:</t>
   </si>
 </sst>
 </file>
@@ -547,87 +547,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Problem Scale'!$I$4:$I$29</c:f>
+              <c:f>'Problem Scale'!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.5141464840000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6465123290000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.8888035889999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.1863854979999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.1155761719999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.6742490229999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.9056552730000007</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13.941623047</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18.335865234</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>24.529195312999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>31.386851563</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41.593425781000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>51.811347656000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>65.555007813000003</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>81.061992188000005</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>98.289351562999997</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>120.353351563</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>144.46899999999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>174.66145312500001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>215.19103125000001</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>273.65828125000002</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>346.10393749999997</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>435.43337500000001</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>553.20487500000002</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>708.90762500000005</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>916.73137499999996</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -857,11 +782,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="350406680"/>
-        <c:axId val="350413736"/>
+        <c:axId val="214998360"/>
+        <c:axId val="215820904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="350406680"/>
+        <c:axId val="214998360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,13 +915,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350413736"/>
+        <c:crossAx val="215820904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="18"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350413736"/>
+        <c:axId val="215820904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1104,7 +1029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350406680"/>
+        <c:crossAx val="214998360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1366,54 +1291,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'~Neighbourhood Scale'!$J$4:$J$18</c:f>
+              <c:f>'~Neighbourhood Scale'!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.7817329099999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.078756592</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.3511909179999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.3128330080000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.7136484379999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.0065546879999996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.513123047000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12.476560547</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15.660400391</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19.406080077999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>18.544294921999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>18.357056641</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>23.299552733999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>23.428734375000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>24.322919922000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1577,11 +1460,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="350405504"/>
-        <c:axId val="350412168"/>
+        <c:axId val="127736320"/>
+        <c:axId val="127411016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="350405504"/>
+        <c:axId val="127736320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1710,13 +1593,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350412168"/>
+        <c:crossAx val="127411016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="18"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350412168"/>
+        <c:axId val="127411016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1824,7 +1707,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350405504"/>
+        <c:crossAx val="127736320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1955,6 +1838,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2108,36 +1992,12 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Entropy!$J$4:$J$12</c:f>
+              <c:f>Entropy!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.78130944800000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.76337078899999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.77297155799999995</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.75933013900000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.76136505099999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.77788977100000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.77518804900000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.75468469199999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.74390893599999997</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2229,11 +2089,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="350409816"/>
-        <c:axId val="350416872"/>
+        <c:axId val="215575976"/>
+        <c:axId val="215576360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="350409816"/>
+        <c:axId val="215575976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,6 +2155,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2361,13 +2222,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350416872"/>
+        <c:crossAx val="215576360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="18"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350416872"/>
+        <c:axId val="215576360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2414,6 +2275,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2474,7 +2336,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350409816"/>
+        <c:crossAx val="215575976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2498,6 +2360,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4341,16 +4204,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>260350</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>574675</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4376,16 +4239,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>231775</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4712,7 +4575,7 @@
   <dimension ref="A2:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4724,7 +4587,7 @@
     <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
-    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -4794,7 +4657,7 @@
         <v>1250</v>
       </c>
       <c r="I4">
-        <v>1.5141464840000001</v>
+        <v>1.3360000000000001</v>
       </c>
       <c r="J4">
         <v>4.8979999999999997</v>
@@ -4830,7 +4693,7 @@
         <v>2160</v>
       </c>
       <c r="I5">
-        <v>1.6465123290000001</v>
+        <v>1.431</v>
       </c>
       <c r="J5">
         <v>9.0640000000000001</v>
@@ -4866,7 +4729,7 @@
         <v>3430</v>
       </c>
       <c r="I6">
-        <v>1.8888035889999999</v>
+        <v>1.575</v>
       </c>
       <c r="J6">
         <v>16.052999</v>
@@ -4902,7 +4765,7 @@
         <v>5120</v>
       </c>
       <c r="I7">
-        <v>3.1863854979999999</v>
+        <v>2.0129999999999999</v>
       </c>
       <c r="J7">
         <v>25.257000000000001</v>
@@ -4938,7 +4801,7 @@
         <v>7290</v>
       </c>
       <c r="I8">
-        <v>5.1155761719999999</v>
+        <v>2.6749999999999998</v>
       </c>
       <c r="J8">
         <v>38.141998000000001</v>
@@ -4974,7 +4837,7 @@
         <v>10000</v>
       </c>
       <c r="I9">
-        <v>7.6742490229999998</v>
+        <v>3.2410000000000001</v>
       </c>
       <c r="J9">
         <v>53.523997999999999</v>
@@ -5010,7 +4873,7 @@
         <v>13310</v>
       </c>
       <c r="I10">
-        <v>8.9056552730000007</v>
+        <v>3.536</v>
       </c>
       <c r="J10">
         <v>69.824996999999996</v>
@@ -5046,7 +4909,7 @@
         <v>17280</v>
       </c>
       <c r="I11">
-        <v>13.941623047</v>
+        <v>4.8689999999999998</v>
       </c>
       <c r="J11">
         <v>93.632003999999995</v>
@@ -5082,7 +4945,7 @@
         <v>21970</v>
       </c>
       <c r="I12">
-        <v>18.335865234</v>
+        <v>5.8</v>
       </c>
       <c r="J12">
         <v>124.17600299999999</v>
@@ -5118,7 +4981,7 @@
         <v>27440</v>
       </c>
       <c r="I13">
-        <v>24.529195312999999</v>
+        <v>7.056</v>
       </c>
       <c r="J13">
         <v>161.74099699999999</v>
@@ -5154,7 +5017,7 @@
         <v>33750</v>
       </c>
       <c r="I14">
-        <v>31.386851563</v>
+        <v>8.202</v>
       </c>
       <c r="J14">
         <v>208.134995</v>
@@ -5190,7 +5053,7 @@
         <v>40960</v>
       </c>
       <c r="I15">
-        <v>41.593425781000001</v>
+        <v>9.8759999999999994</v>
       </c>
       <c r="J15">
         <v>276.60400399999997</v>
@@ -5226,7 +5089,7 @@
         <v>49130</v>
       </c>
       <c r="I16">
-        <v>51.811347656000002</v>
+        <v>11.509</v>
       </c>
       <c r="J16">
         <v>369.57998700000002</v>
@@ -5262,7 +5125,7 @@
         <v>58320</v>
       </c>
       <c r="I17">
-        <v>65.555007813000003</v>
+        <v>13.494</v>
       </c>
       <c r="J17">
         <v>491.15100100000001</v>
@@ -5298,7 +5161,7 @@
         <v>68590</v>
       </c>
       <c r="I18">
-        <v>81.061992188000005</v>
+        <v>15.542999999999999</v>
       </c>
       <c r="J18">
         <v>675.02899200000002</v>
@@ -5334,7 +5197,7 @@
         <v>80000</v>
       </c>
       <c r="I19">
-        <v>98.289351562999997</v>
+        <v>17.913</v>
       </c>
       <c r="J19">
         <v>892.57098399999995</v>
@@ -5370,7 +5233,7 @@
         <v>92610</v>
       </c>
       <c r="I20">
-        <v>120.353351563</v>
+        <v>22.693000000000001</v>
       </c>
       <c r="J20">
         <v>1121.4079589999999</v>
@@ -5406,7 +5269,7 @@
         <v>106480</v>
       </c>
       <c r="I21">
-        <v>144.46899999999999</v>
+        <v>25.920999999999999</v>
       </c>
       <c r="J21">
         <v>1443.1739500000001</v>
@@ -5442,7 +5305,7 @@
         <v>121670</v>
       </c>
       <c r="I22">
-        <v>174.66145312500001</v>
+        <v>30.81</v>
       </c>
       <c r="J22">
         <v>1775.485962</v>
@@ -5478,7 +5341,7 @@
         <v>138240</v>
       </c>
       <c r="I23">
-        <v>215.19103125000001</v>
+        <v>39.148000000000003</v>
       </c>
       <c r="J23">
         <v>2107.0339359999998</v>
@@ -5514,7 +5377,7 @@
         <v>156250</v>
       </c>
       <c r="I24">
-        <v>273.65828125000002</v>
+        <v>51.165999999999997</v>
       </c>
       <c r="J24">
         <v>2752.3911130000001</v>
@@ -5550,7 +5413,7 @@
         <v>175760</v>
       </c>
       <c r="I25">
-        <v>346.10393749999997</v>
+        <v>64.558999999999997</v>
       </c>
       <c r="J25">
         <v>3156.6499020000001</v>
@@ -5586,7 +5449,7 @@
         <v>196830</v>
       </c>
       <c r="I26">
-        <v>435.43337500000001</v>
+        <v>83.641999999999996</v>
       </c>
       <c r="J26">
         <v>3492.8930660000001</v>
@@ -5622,7 +5485,7 @@
         <v>219520</v>
       </c>
       <c r="I27">
-        <v>553.20487500000002</v>
+        <v>106.489</v>
       </c>
       <c r="J27">
         <v>4196.5161129999997</v>
@@ -5658,7 +5521,7 @@
         <v>243890</v>
       </c>
       <c r="I28">
-        <v>708.90762500000005</v>
+        <v>128.84200000000001</v>
       </c>
       <c r="J28">
         <v>4713.9858400000003</v>
@@ -5694,7 +5557,7 @@
         <v>270000</v>
       </c>
       <c r="I29">
-        <v>916.73137499999996</v>
+        <v>157.709</v>
       </c>
       <c r="J29">
         <v>5139.0390630000002</v>
@@ -5709,7 +5572,7 @@
       </c>
       <c r="I31">
         <f>PEARSON(H4:H29,I4:I29)</f>
-        <v>0.94983175514954699</v>
+        <v>0.95379491839273389</v>
       </c>
       <c r="J31">
         <f>PEARSON(H4:H29,J4:J29)</f>
@@ -5725,8 +5588,8 @@
         <v>15</v>
       </c>
       <c r="I32">
-        <f>PEARSON(H24:H29,I24:I29)</f>
-        <v>0.98995036505789602</v>
+        <f>PEARSON(H21:H29,I21:I29)</f>
+        <v>0.99079914770659683</v>
       </c>
     </row>
     <row r="34" spans="8:9" x14ac:dyDescent="0.25">
@@ -5929,8 +5792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:J21"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6020,7 +5883,7 @@
         <v>0.25132741228718347</v>
       </c>
       <c r="J4">
-        <v>1.7817329099999999</v>
+        <v>1.615</v>
       </c>
       <c r="K4">
         <v>11.044</v>
@@ -6060,7 +5923,7 @@
         <v>2.0106192982974678</v>
       </c>
       <c r="J5">
-        <v>2.078756592</v>
+        <v>1.446</v>
       </c>
       <c r="K5">
         <v>17.268999000000001</v>
@@ -6100,7 +5963,7 @@
         <v>6.7858401317539538</v>
       </c>
       <c r="J6">
-        <v>3.3511909179999999</v>
+        <v>1.6619999999999999</v>
       </c>
       <c r="K6">
         <v>27.846001000000001</v>
@@ -6140,7 +6003,7 @@
         <v>16.084954386379742</v>
       </c>
       <c r="J7">
-        <v>5.3128330080000001</v>
+        <v>2.3610000000000002</v>
       </c>
       <c r="K7">
         <v>38.735000999999997</v>
@@ -6180,7 +6043,7 @@
         <v>31.415926535897935</v>
       </c>
       <c r="J8">
-        <v>7.7136484379999999</v>
+        <v>3.4990000000000001</v>
       </c>
       <c r="K8">
         <v>53.648997999999999</v>
@@ -6220,7 +6083,7 @@
         <v>54.286721054031631</v>
       </c>
       <c r="J9">
-        <v>9.0065546879999996</v>
+        <v>4.0350000000000001</v>
       </c>
       <c r="K9">
         <v>72.196999000000005</v>
@@ -6260,7 +6123,7 @@
         <v>86.205302414503933</v>
       </c>
       <c r="J10">
-        <v>10.513123047000001</v>
+        <v>5.5179999999999998</v>
       </c>
       <c r="K10">
         <v>95.566001999999997</v>
@@ -6300,7 +6163,7 @@
         <v>128.67963509103794</v>
       </c>
       <c r="J11">
-        <v>12.476560547</v>
+        <v>7.4640000000000004</v>
       </c>
       <c r="K11">
         <v>122.63200399999999</v>
@@ -6340,7 +6203,7 @@
         <v>183.21768355735676</v>
       </c>
       <c r="J12">
-        <v>15.660400391</v>
+        <v>10.64</v>
       </c>
       <c r="K12">
         <v>146.36000100000001</v>
@@ -6380,7 +6243,7 @@
         <v>251.32741228718348</v>
       </c>
       <c r="J13">
-        <v>19.406080077999999</v>
+        <v>17.864999999999998</v>
       </c>
       <c r="K13">
         <v>189.804993</v>
@@ -6420,7 +6283,7 @@
         <v>334.5167857542412</v>
       </c>
       <c r="J14">
-        <v>18.544294921999999</v>
+        <v>18.125</v>
       </c>
       <c r="K14">
         <v>235.32600400000001</v>
@@ -6460,7 +6323,7 @@
         <v>434.29376843225305</v>
       </c>
       <c r="J15">
-        <v>18.357056641</v>
+        <v>18.231000000000002</v>
       </c>
       <c r="K15">
         <v>267.49301100000002</v>
@@ -6500,7 +6363,7 @@
         <v>552.16632479494206</v>
       </c>
       <c r="J16">
-        <v>23.299552733999999</v>
+        <v>31.797000000000001</v>
       </c>
       <c r="K16">
         <v>346.46099900000002</v>
@@ -6540,7 +6403,7 @@
         <v>689.64241931603146</v>
       </c>
       <c r="J17">
-        <v>23.428734375000001</v>
+        <v>32.146000000000001</v>
       </c>
       <c r="K17">
         <v>375.97601300000002</v>
@@ -6580,7 +6443,7 @@
         <v>848.23001646924422</v>
       </c>
       <c r="J18">
-        <v>24.322919922000001</v>
+        <v>32.932000000000002</v>
       </c>
       <c r="K18">
         <v>412.51199300000002</v>
@@ -6595,7 +6458,7 @@
       </c>
       <c r="J20">
         <f>PEARSON(I4:I18,J4:J18)</f>
-        <v>0.90496685194058868</v>
+        <v>0.97361612871523606</v>
       </c>
       <c r="K20">
         <f>PEARSON(I4:I18,K4:K18)</f>
@@ -6736,8 +6599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6819,7 +6682,7 @@
         <v>31.415926535897935</v>
       </c>
       <c r="J4">
-        <v>0.78130944800000002</v>
+        <v>0.35</v>
       </c>
       <c r="K4">
         <v>5.6310000000000002</v>
@@ -6859,7 +6722,7 @@
         <v>31.415926535897935</v>
       </c>
       <c r="J5">
-        <v>0.76337078899999999</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="K5">
         <v>5.5529999999999999</v>
@@ -6899,7 +6762,7 @@
         <v>31.415926535897935</v>
       </c>
       <c r="J6">
-        <v>0.77297155799999995</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="K6">
         <v>5.444</v>
@@ -6939,7 +6802,7 @@
         <v>31.415926535897935</v>
       </c>
       <c r="J7">
-        <v>0.75933013900000002</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="K7">
         <v>5.4909999999999997</v>
@@ -6979,7 +6842,7 @@
         <v>31.415926535897935</v>
       </c>
       <c r="J8">
-        <v>0.76136505099999996</v>
+        <v>0.36</v>
       </c>
       <c r="K8">
         <v>5.5839999999999996</v>
@@ -7019,7 +6882,7 @@
         <v>31.415926535897935</v>
       </c>
       <c r="J9">
-        <v>0.77788977100000001</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="K9">
         <v>5.6310000000000002</v>
@@ -7059,7 +6922,7 @@
         <v>31.415926535897935</v>
       </c>
       <c r="J10">
-        <v>0.77518804900000005</v>
+        <v>0.36</v>
       </c>
       <c r="K10">
         <v>5.57</v>
@@ -7099,7 +6962,7 @@
         <v>31.415926535897935</v>
       </c>
       <c r="J11">
-        <v>0.75468469199999999</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="K11">
         <v>5.4909999999999997</v>
@@ -7139,7 +7002,7 @@
         <v>31.415926535897935</v>
       </c>
       <c r="J12">
-        <v>0.74390893599999997</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="K12">
         <v>5.5069999999999997</v>

</xml_diff>